<commit_message>
correção testes de integração de autenticação e melhoria na leitura dos arquivos excel
</commit_message>
<xml_diff>
--- a/src/test/resources/student.xlsx
+++ b/src/test/resources/student.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>RA</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>gabriela.lisboa@fatec.sp.gov.br</t>
+  </si>
+  <si>
+    <t>Paulo Coelho Souza</t>
+  </si>
+  <si>
+    <t>paulo.souza@fatec.sp.gov.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -412,16 +424,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -466,6 +478,34 @@
       </c>
       <c r="D3" s="5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1460311714078</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1239665691</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>